<commit_message>
updates to build dashboard
</commit_message>
<xml_diff>
--- a/ReportingDashboardExport.xlsx
+++ b/ReportingDashboardExport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rpxcorp-my.sharepoint.com/personal/jmiller_rpxcorp_com/Documents/R Projects/Reporting Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="184" documentId="13_ncr:1_{C0542016-DE8A-475F-A906-0E4C75787925}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B87A8C0A-492D-4E84-932D-937A385BC09F}"/>
+  <xr:revisionPtr revIDLastSave="187" documentId="13_ncr:1_{C0542016-DE8A-475F-A906-0E4C75787925}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6F6C996E-59D8-417A-922E-AF38CA35DFD6}"/>
   <bookViews>
-    <workbookView xWindow="53652" yWindow="-1764" windowWidth="30936" windowHeight="16896" tabRatio="678" xr2:uid="{20B6C54F-D2F3-42DB-A199-C302E528B8D6}"/>
+    <workbookView xWindow="22932" yWindow="-1692" windowWidth="30936" windowHeight="16896" tabRatio="678" activeTab="2" xr2:uid="{20B6C54F-D2F3-42DB-A199-C302E528B8D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Defs Added by Quarter" sheetId="1" r:id="rId1"/>
@@ -1779,7 +1779,7 @@
       <c:catAx>
         <c:axId val="886196816"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1827,7 +1827,7 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
-        <c:axPos val="b"/>
+        <c:axPos val="t"/>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2184,7 +2184,7 @@
       <c:catAx>
         <c:axId val="886196816"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2232,7 +2232,7 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
-        <c:axPos val="b"/>
+        <c:axPos val="t"/>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2582,7 +2582,7 @@
       <c:catAx>
         <c:axId val="874420072"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2630,7 +2630,7 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
-        <c:axPos val="b"/>
+        <c:axPos val="t"/>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -8940,7 +8940,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53F5D069-C005-4D7F-87B6-6C19F6DA410E}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9870,7 +9872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C6910EE-80BC-431D-B158-4F66462A430E}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>